<commit_message>
results for gpt 3.5 and gpt4(level 1 to 8 only)
</commit_message>
<xml_diff>
--- a/graph_generation/results_prelim/gpt3.5/level_1/k_0.xlsx
+++ b/graph_generation/results_prelim/gpt3.5/level_1/k_0.xlsx
@@ -8,13 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="o_10" sheetId="1" r:id="rId1"/>
+    <sheet name="o_20" sheetId="2" r:id="rId2"/>
+    <sheet name="o_20_jumbled" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>prompt</t>
   </si>
@@ -26,6 +28,9 @@
   </si>
   <si>
     <t>evaluator_response</t>
+  </si>
+  <si>
+    <t>evaluator_partial_correctness</t>
   </si>
   <si>
     <t xml:space="preserve"> Given is the adjacency matrix for a unweighted undirected graph containing 10 nodes labelled A to J. The value corresponding to each row M and column N represents whether there is a connection between the two nodes, where 0 means no connection.   
@@ -47,22 +52,93 @@
     <t>A -&gt; B -&gt; C -&gt; D -&gt; E -&gt; F -&gt; G -&gt; H -&gt; I -&gt; J</t>
   </si>
   <si>
-    <t>To find the shortest path from node A to node J, we can use Dijkstra's algorithm.
-1. Initialize a distance array to keep track of the shortest distance from node A to each node. Set the distance from A to A as 0 and all other distances as infinity.
-   Distance: [0, infinity, infinity, infinity, infinity, infinity, infinity, infinity, infinity, infinity]
-2. Create a set called unvisited to keep track of the unvisited nodes. Initially, add all nodes to the unvisited set.
-   Unvisited: [A, B, C, D, E, F, G, H, I, J]
-3. While the unvisited set is not empty:
-   a. Find the node with the minimum distance from A in the distance array. Let's call this node current.
-   b. Remove current from the unvisited set.
-   c. For each neighbor of current that is still in the unvisited set, calculate the distance from A to the neighbor through current. If this distance is smaller than the current distance in the distance array, update the distance array.
-   The algorithm continues until the unvisited set is empty.
-4. After running Dijkstra's algorithm using the given adjacency matrix, the final distance array would be:
-   Distance: [0, 1, 2, 3, 4, 5, 6, 7, 8, 9]
-So, the shortest path from node A to node J is A -&gt; B -&gt; C -&gt; D -&gt; E -&gt; F -&gt; G -&gt; H -&gt; I -&gt; J.</t>
-  </si>
-  <si>
-    <t>Correct</t>
+    <t>To find the shortest path from node A to node J, we can use the breadth-first search (BFS) algorithm.
+Starting from node A, we explore all its neighboring nodes (nodes B and C). Then, we explore the neighboring nodes of B and C, and continue this process until we reach node J.
+The steps to find the shortest path are as follows:
+1. Create an empty queue and enqueue node A.
+2. Create an empty visited set to keep track of visited nodes.
+3. Create an empty parent dictionary to store the parent node for each visited node.
+4. While the queue is not empty, do the following:
+   - Dequeue a node from the queue.
+   - If the dequeued node is node J, we have found the shortest path.
+   - Otherwise, for each neighboring node of the dequeued node that has not been visited, do the following:
+     - Enqueue the neighboring node.
+     - Mark the neighboring node as visited.
+     - Set the parent of the neighboring node as the dequeued node in the parent dictionary.
+5. If we have reached this step, it means that there is no path from node A to node J.
+Using the adjacency matrix provided, we can implement the BFS algorithm to find the shortest path from node A to node J.</t>
+  </si>
+  <si>
+    <t>Wrong</t>
+  </si>
+  <si>
+    <t>Output: 0/10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Given is the adjacency matrix for a unweighted undirected graph containing 20 nodes labelled A to T. The value corresponding to each row M and column N represents whether there is a connection between the two nodes, where 0 means no connection.   
+what is the shortest path from node A to node T?
+   A B C D E F G H I J K L M N O P Q R S T
+ A 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ B 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ C 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ D 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ E 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0 0
+ F 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0 0
+ G 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0 0
+ H 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0 0
+ I 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0 0
+ J 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0 0
+ K 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0 0
+ L 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0 0
+ M 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0 0
+ N 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0 0
+ O 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0 0
+ P 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0 0
+ Q 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0 0
+ R 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1 0
+ S 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0 1
+ T 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 0 1 0
+    </t>
+  </si>
+  <si>
+    <t>A -&gt; B -&gt; C -&gt; D -&gt; E -&gt; F -&gt; G -&gt; H -&gt; I -&gt; J -&gt; K -&gt; L -&gt; M -&gt; N -&gt; O -&gt; P -&gt; Q -&gt; R -&gt; S -&gt; T</t>
+  </si>
+  <si>
+    <t>To find the shortest path from node A to node T, we can use Dijkstra's algorithm.
+1. Initialize an array `dist` with size 20 to keep track of the shortest distance from node A to each other node. Start by setting the distance from A to A as 0 and the distance from A to all other nodes as infinity.
+   dist = [0, ∞, ∞, ∞, ∞, ∞, ∞, ∞, ∞, ∞, ∞, ∞, ∞, ∞, ∞, ∞, ∞, ∞, ∞, ∞]
+2. Initialize a set `visited` to keep track of the nodes we have visited. Start by adding node A to the set.
+   visited = {A}
+3. While the set `visited` does not contain all nodes:
+   - Find the node `u` in the set `visited` with the minimum distance from node A. This can be done by iterating through all nodes in the set and selecting the node with the minimum value in the `dist` array.
+   - Add the node `u` to the set of visited nodes.
+   - For each neighbor `v` of `u` that is not in the set `visited`:
+     - Calculate the new distance `new_dist` from node A to `v` through `u` by adding the value in the adjacency matrix for the connection between `u` and `v` to the distance from A to `u`.
+     - If `new_dist` is smaller than the current distance in the `dist` array for node `v`, update the `dist` array with the new distance.
+4. After the algorithm terminates, the shortest distance from node A to node T will be the value in the `dist` array for node T.
+In this case, the shortest path from node A to node T has a distance of 2.
+Note: The actual path from node A to node T will depend on the actual connections between the nodes in the graph.</t>
+  </si>
+  <si>
+    <t>Output: 1/20</t>
+  </si>
+  <si>
+    <t>To find the shortest path from node A to node T, we can use Dijkstra's algorithm. 
+1. Start by setting the distance from node A to itself as 0, and all other distances as infinity. 
+   - Distance[A] = 0
+   - Distance[B] = infinity
+   - Distance[C] = infinity
+   ...
+   - Distance[T] = infinity
+2. Set the current node as A and mark it as visited. 
+3. For each neighbor of the current node, calculate the distance from A to that neighbor through the current node. If this distance is shorter than the previously recorded distance for that neighbor, update it. 
+   - For example, if current node is A and the neighbor is B: 
+     - Distance[B] = min(Distance[B], Distance[A] + 1) = min(infinity, 0 + 1) = 1
+   - Repeat this for all neighbors of the current node. 
+4. Once all neighbors of the current node have been updated, mark the current node as visited. 
+5. Select the unvisited node with the smallest distance as the new current node and repeat steps 3 to 5 until the destination node (T) is visited. 
+6. The shortest path from A to T can be found by backtracking from T to A using the recorded distances. 
+The step-by-step application of Dijkstra's algorithm to find the shortest path from A to T may be quite extensive to describe. Please let me know if a more detailed explanation is required.</t>
   </si>
 </sst>
 </file>
@@ -420,13 +496,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,19 +515,119 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>